<commit_message>
Added onltology to demo graph
</commit_message>
<xml_diff>
--- a/infra/demo/equipment.xlsx
+++ b/infra/demo/equipment.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\repos\simple-digital-twin\infra\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\repos\simple-digital-twin\infra\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1EC0BE1F-8876-418C-9F58-1A71D509F0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FB0577-D28A-4385-9CD9-7191C263910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="23385" activeTab="1"/>
+    <workbookView xWindow="16095" yWindow="-20460" windowWidth="38700" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
     <sheet name="Relationships" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>class</t>
   </si>
@@ -89,112 +102,115 @@
     <t>pipe3</t>
   </si>
   <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>boundary</t>
+  </si>
+  <si>
+    <t>anchor</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>isin</t>
+  </si>
+  <si>
+    <t>connects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:anchor;1</t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:anchor;2</t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:anchor;3</t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:anchor;4</t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:anchor;5</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>anchor1</t>
+  </si>
+  <si>
+    <t>anchor2</t>
+  </si>
+  <si>
+    <t>anchor3</t>
+  </si>
+  <si>
+    <t>anchor4</t>
+  </si>
+  <si>
+    <t>anchor5</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:area;1</t>
+  </si>
+  <si>
+    <t>dtmi:billmanh:asset;1</t>
+  </si>
+  <si>
+    <t>pnid1</t>
+  </si>
+  <si>
+    <t>facility1</t>
+  </si>
+  <si>
+    <t>storage_type</t>
+  </si>
+  <si>
+    <t>storage_path</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>azureblob</t>
+  </si>
+  <si>
+    <t>static/assets/pnid1.png</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
-    <t>asset</t>
-  </si>
-  <si>
-    <t>boundary</t>
-  </si>
-  <si>
-    <t>anchor</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>isin</t>
-  </si>
-  <si>
-    <t>connects</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;1</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;2</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;3</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;4</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;5</t>
-  </si>
-  <si>
-    <t>has</t>
-  </si>
-  <si>
-    <t>anchor1</t>
-  </si>
-  <si>
-    <t>anchor2</t>
-  </si>
-  <si>
-    <t>anchor3</t>
-  </si>
-  <si>
-    <t>anchor4</t>
-  </si>
-  <si>
-    <t>anchor5</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:area;1</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:asset;1</t>
-  </si>
-  <si>
-    <t>pnid1</t>
-  </si>
-  <si>
-    <t>facility1</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>storage_type</t>
-  </si>
-  <si>
-    <t>storage_path</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>png</t>
-  </si>
-  <si>
-    <t>azureblob</t>
-  </si>
-  <si>
-    <t>static/assets/pnid1.png</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
+    <t>boundary1</t>
+  </si>
+  <si>
+    <t>local_x</t>
+  </si>
+  <si>
+    <t>local_y</t>
+  </si>
+  <si>
+    <t>local_z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1034,35 +1050,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1101,25 +1117,25 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
       <c r="Q1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="R1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1154,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1189,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1227,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1265,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1303,18 +1319,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q7">
         <v>10</v>
@@ -1326,18 +1342,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q8">
         <v>20</v>
@@ -1349,18 +1365,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q9">
         <v>30</v>
@@ -1372,18 +1388,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q10">
         <v>-10</v>
@@ -1395,18 +1411,18 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q11">
         <v>50</v>
@@ -1418,29 +1434,32 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
       <c r="D12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1452,32 +1471,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
       <c r="N14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1488,29 +1507,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1519,9 +1538,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1530,9 +1549,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1541,9 +1560,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1552,9 +1571,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1563,9 +1582,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1574,9 +1593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1585,9 +1604,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1596,9 +1615,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1607,9 +1626,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1618,9 +1637,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1629,9 +1648,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1640,9 +1659,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -1651,9 +1670,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1662,9 +1681,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1673,9 +1692,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>13</v>
@@ -1687,4 +1706,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{5fae8262-b78e-4366-8929-a5d6aac95320}" enabled="1" method="Standard" siteId="{cf36141c-ddd7-45a7-b073-111f66d0b30c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update to gh build file
</commit_message>
<xml_diff>
--- a/infra/demo/equipment.xlsx
+++ b/infra/demo/equipment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\repos\simple-digital-twin\infra\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\repos\simple-digital-twin\infra\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79853A8-0661-4018-80FA-C40E78C823AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0F3629-D5A7-4B37-9F28-73274F3528A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
   <si>
     <t>class</t>
   </si>
@@ -75,33 +75,12 @@
     <t>tank</t>
   </si>
   <si>
-    <t>dtmi:billmanh:tank;1</t>
-  </si>
-  <si>
-    <t>large_tank</t>
-  </si>
-  <si>
     <t>ACME</t>
   </si>
   <si>
-    <t>small_tank</t>
-  </si>
-  <si>
     <t>pipe</t>
   </si>
   <si>
-    <t>dtmi:billmanh:pipe;1</t>
-  </si>
-  <si>
-    <t>pipe1</t>
-  </si>
-  <si>
-    <t>pipe2</t>
-  </si>
-  <si>
-    <t>pipe3</t>
-  </si>
-  <si>
     <t>asset</t>
   </si>
   <si>
@@ -126,54 +105,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>dtmi:billmanh:anchor;1</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;2</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;3</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;4</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:anchor;5</t>
-  </si>
-  <si>
     <t>has</t>
   </si>
   <si>
-    <t>anchor1</t>
-  </si>
-  <si>
-    <t>anchor2</t>
-  </si>
-  <si>
-    <t>anchor3</t>
-  </si>
-  <si>
-    <t>anchor4</t>
-  </si>
-  <si>
-    <t>anchor5</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
-    <t>dtmi:billmanh:area;1</t>
-  </si>
-  <si>
-    <t>dtmi:billmanh:asset;1</t>
-  </si>
-  <si>
-    <t>pnid1</t>
-  </si>
-  <si>
-    <t>facility1</t>
-  </si>
-  <si>
     <t>storage_type</t>
   </si>
   <si>
@@ -195,9 +132,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>boundary1</t>
-  </si>
-  <si>
     <t>local_x</t>
   </si>
   <si>
@@ -205,6 +139,63 @@
   </si>
   <si>
     <t>local_z</t>
+  </si>
+  <si>
+    <t>workorder</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>display_name</t>
+  </si>
+  <si>
+    <t>Large Storage Tank</t>
+  </si>
+  <si>
+    <t>Small Staging Tank</t>
+  </si>
+  <si>
+    <t>Large Tank Egress Pipe</t>
+  </si>
+  <si>
+    <t>Small Tank Ingress Pipe</t>
+  </si>
+  <si>
+    <t>Small Tank to large Tank Return</t>
+  </si>
+  <si>
+    <t>Main Processing Facility</t>
+  </si>
+  <si>
+    <t>Piping and Infrastructure Diagram</t>
+  </si>
+  <si>
+    <t>Cleaning Order</t>
+  </si>
+  <si>
+    <t>Stress Test</t>
+  </si>
+  <si>
+    <t>Valve Reset</t>
+  </si>
+  <si>
+    <t>Pretty Good Tank Cleaning LLC</t>
+  </si>
+  <si>
+    <t>Pipe and Valve Maintenance CO, West</t>
+  </si>
+  <si>
+    <t>Large Tank Management and Cleaning</t>
+  </si>
+  <si>
+    <t>Small Tank Processes and Maintenance</t>
+  </si>
+  <si>
+    <t>Pipe Management for Dummies</t>
   </si>
 </sst>
 </file>
@@ -1051,34 +1042,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1087,416 +1080,694 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" t="s">
-        <v>47</v>
-      </c>
       <c r="P1" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="Q1" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="R1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="S1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="str">
+        <f>"dtmi:billmanh:"&amp;B2&amp;";1"</f>
+        <v>dtmi:billmanh:tank;1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="str">
+        <f>B2&amp;"_"&amp;A2</f>
+        <v>tank_1</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
+      <c r="H2">
         <v>1234</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>500</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>500</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C26" si="0">"dtmi:billmanh:"&amp;B3&amp;";1"</f>
+        <v>dtmi:billmanh:tank;1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E26" si="1">B3&amp;"_"&amp;A3</f>
+        <v>tank_2</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3">
+      <c r="H3">
         <v>1234</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>200</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:pipe;1</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4">
+        <v>41</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>pipe_3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
         <v>2345</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:pipe;1</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
+        <v>42</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>pipe_4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
         <v>2345</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
       </c>
       <c r="I5">
         <v>10</v>
       </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:pipe;1</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6">
+        <v>43</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>pipe_5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
         <v>2345</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7">
-        <v>10</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:anchor;1</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>anchor_6</v>
       </c>
       <c r="S7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8">
-        <v>20</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:anchor;1</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>anchor_7</v>
       </c>
       <c r="S8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9">
-        <v>30</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:anchor;1</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>anchor_8</v>
       </c>
       <c r="S9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10">
-        <v>-10</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:anchor;1</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>anchor_9</v>
       </c>
       <c r="S10">
         <v>-10</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11">
-        <v>50</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:anchor;1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>anchor_10</v>
       </c>
       <c r="S11">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:area;1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>area_11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:boundary;1</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>boundary_12</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:asset;1</v>
+      </c>
+      <c r="D14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>asset_13</v>
+      </c>
+      <c r="P14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="str">
+        <f>"dtmi:billmanh:"&amp;B15&amp;";1"</f>
+        <v>dtmi:billmanh:workorder;1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>workorder_14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:workorder;1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>workorder_15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:workorder;1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>workorder_16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:workorder;1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>workorder_17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:workorder;1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>workorder_18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:vendor;1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>vendor_19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:vendor;1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>vendor_20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:document;1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>document_21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:document;1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>document_22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:document;1</v>
+      </c>
+      <c r="D24" t="s">
         <v>53</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>document_23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:document;1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>document_24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>dtmi:billmanh:document;1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>document_25</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
         <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="N14" t="s">
-        <v>50</v>
-      </c>
-      <c r="O14" t="s">
-        <v>51</v>
-      </c>
-      <c r="P14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1510,26 +1781,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1538,9 +1809,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1549,9 +1820,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1560,9 +1831,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1571,9 +1842,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1582,9 +1853,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1593,9 +1864,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1604,9 +1875,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1615,9 +1886,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1626,9 +1897,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -1637,9 +1908,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1648,9 +1919,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1659,9 +1930,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -1670,9 +1941,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1681,9 +1952,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1692,9 +1963,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>13</v>
@@ -1703,9 +1974,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -1714,9 +1985,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>7</v>
@@ -1725,9 +1996,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1736,9 +2007,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>9</v>
@@ -1747,9 +2018,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>10</v>

</xml_diff>